<commit_message>
Update dependencies and enhance StockForm component with search functionality. Added new dependencies for QR code generation and ESLint plugins, updated existing packages, and refactored StockForm to include a search bar for stock cards. Improved error handling and form state management, ensuring a better user experience when managing stock items.
</commit_message>
<xml_diff>
--- a/public/stock_card_import.xlsx
+++ b/public/stock_card_import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Eren/erp-ims/erp-dev-frontend/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C132E590-C9F2-FE47-A59F-EF2540F81BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6DB03059-676B-084C-8893-D39E830685D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>productCode</t>
   </si>
@@ -110,46 +110,58 @@
     <t>BasitUrun</t>
   </si>
   <si>
-    <t>REMA/iP-15ProMax/Siyah</t>
-  </si>
-  <si>
-    <t>Apple Iphone 15 Pro Max Magsafe Wireless Şarj Özellikli Silikon 2mm Kamera Çıkıntılı Rema Kılıf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rema Iphone 15 Pro Max </t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>B1</t>
-  </si>
-  <si>
-    <t>Brand 1</t>
-  </si>
-  <si>
     <t>Rema Kılıf</t>
   </si>
   <si>
-    <t>Renk=Siyah,Cihaz Modeli=iPhone 15 Pro Max</t>
-  </si>
-  <si>
-    <t>Ege</t>
-  </si>
-  <si>
-    <t>Tip 1 Bayiler=1,Tip 2 Bayiler=1,5,Tip 3 Bayiler=3,Perakende=100,E-Ticaret=200</t>
-  </si>
-  <si>
     <t>warehouseName</t>
   </si>
   <si>
     <t>quantity</t>
   </si>
   <si>
-    <t>Ana Depo</t>
-  </si>
-  <si>
-    <t>8683603022727,1</t>
+    <t>REMA/iP-11/AçıkMavi</t>
+  </si>
+  <si>
+    <t>Apple Iphone 11 Magsafe Wireless Şarj Özellikli Silikon 2mm Kamera Çıkıntılı Rema Kılıf</t>
+  </si>
+  <si>
+    <t>Renk=Açık Mavi,Cihaz Modeli=iPhone 11</t>
+  </si>
+  <si>
+    <t>VIP</t>
+  </si>
+  <si>
+    <t>ETC</t>
+  </si>
+  <si>
+    <t>E-Ticaret</t>
+  </si>
+  <si>
+    <t>VipCase</t>
+  </si>
+  <si>
+    <t>REMA iPhone 11 Açık Mavi</t>
+  </si>
+  <si>
+    <t>REMA/iP-11/AçıkMavi,8683606399265</t>
+  </si>
+  <si>
+    <t>EGE</t>
+  </si>
+  <si>
+    <t>Tip 1 Bayiler=1,Tip 2 Bayiler=1.4,Tip 3 Bayiler=1.8,Maliyet=0.8,Perakende=150</t>
+  </si>
+  <si>
+    <t>maliyet</t>
+  </si>
+  <si>
+    <t>maliyetKur</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>vatRate</t>
   </si>
 </sst>
 </file>
@@ -214,11 +226,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,18 +536,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="74.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="75.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.1640625" bestFit="1" customWidth="1"/>
@@ -545,19 +558,21 @@
     <col min="13" max="13" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="40.83203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="61.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12" customWidth="1"/>
+    <col min="18" max="18" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="41.6640625" customWidth="1"/>
+    <col min="25" max="25" width="61.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="41" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -604,57 +619,66 @@
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
         <v>35</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -668,35 +692,47 @@
       <c r="O2">
         <v>50</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2">
+        <v>50</v>
+      </c>
+      <c r="T2" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" t="s">
+        <v>24</v>
+      </c>
+      <c r="V2" t="s">
+        <v>25</v>
+      </c>
+      <c r="W2" t="s">
+        <v>30</v>
+      </c>
+      <c r="X2">
+        <v>20</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB2" t="s">
         <v>37</v>
-      </c>
-      <c r="Q2">
-        <v>100</v>
-      </c>
-      <c r="R2" t="s">
-        <v>30</v>
-      </c>
-      <c r="S2" t="s">
-        <v>24</v>
-      </c>
-      <c r="T2" t="s">
-        <v>31</v>
-      </c>
-      <c r="U2" t="s">
-        <v>32</v>
-      </c>
-      <c r="V2" t="s">
-        <v>34</v>
-      </c>
-      <c r="W2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AB2">
+    <sortCondition ref="A2"/>
+  </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>